<commit_message>
Create Excel list of Import Dependencies
</commit_message>
<xml_diff>
--- a/Calculations/Balance Bot Module Imports.xlsx
+++ b/Calculations/Balance Bot Module Imports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulJ\Data\Science\Engineering\Robotics\Balance_Bot\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF6398F-3918-4E16-A8B5-4FACD7029C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F8C65D-7D5A-4FAA-9661-3F2EBF030D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15916" xr2:uid="{64651FD6-1710-4F20-A6CC-656AB4CC03CF}"/>
+    <workbookView xWindow="12593" yWindow="705" windowWidth="8527" windowHeight="11513" xr2:uid="{64651FD6-1710-4F20-A6CC-656AB4CC03CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="202">
   <si>
     <t>Balance Bot Module Import Requirements</t>
   </si>
@@ -630,6 +630,9 @@
   </si>
   <si>
     <t>pywin32 ?</t>
+  </si>
+  <si>
+    <t>End of Project Module Direct Dependencies</t>
   </si>
 </sst>
 </file>
@@ -671,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -689,6 +692,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,13 +1009,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DF46FB-8718-49D2-B329-E715A5B99079}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C137" sqref="C137"/>
+      <selection pane="bottomRight" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -1051,7 +1057,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1059,7 +1065,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1083,7 +1089,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -1171,7 +1177,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1187,7 +1193,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -1195,7 +1201,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
@@ -1211,7 +1217,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -1227,7 +1233,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -1969,318 +1975,327 @@
         <v>110</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A110" s="7" t="s">
+        <v>201</v>
+      </c>
       <c r="E110" s="3"/>
     </row>
-    <row r="111" spans="1:5" ht="67.5" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" spans="1:5" ht="67.5" x14ac:dyDescent="0.4">
+      <c r="A113" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A112" t="s">
-        <v>68</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E112" s="3"/>
-    </row>
-    <row r="113" spans="1:5" ht="27" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>69</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>132</v>
+        <v>68</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E114" s="3"/>
     </row>
-    <row r="115" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>76</v>
-      </c>
-      <c r="C115" t="s">
-        <v>133</v>
-      </c>
-      <c r="D115" t="s">
-        <v>134</v>
+        <v>69</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="E116" s="3"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C117" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D117" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>79</v>
-      </c>
-      <c r="C118" t="s">
-        <v>141</v>
-      </c>
-      <c r="D118" t="s">
-        <v>142</v>
-      </c>
-      <c r="E118" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C119" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D119" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="C120" t="s">
+        <v>141</v>
+      </c>
+      <c r="D120" t="s">
+        <v>142</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>150</v>
-      </c>
-      <c r="E121" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="C121" t="s">
+        <v>145</v>
+      </c>
+      <c r="D121" t="s">
+        <v>146</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
+        <v>81</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>150</v>
+      </c>
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>82</v>
       </c>
-      <c r="E122" s="3"/>
-    </row>
-    <row r="123" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
-      <c r="A123" t="s">
-        <v>83</v>
-      </c>
-      <c r="E123" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="27" x14ac:dyDescent="0.35">
-      <c r="A124" t="s">
-        <v>84</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="E124" s="3"/>
     </row>
     <row r="125" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
+        <v>83</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="27" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>84</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>144</v>
       </c>
-      <c r="E125" s="3" t="s">
+      <c r="E127" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="67.5" x14ac:dyDescent="0.35">
-      <c r="A126" t="s">
+    <row r="128" spans="1:5" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>85</v>
       </c>
-      <c r="E126" s="3" t="s">
+      <c r="E128" s="3" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="27" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
-        <v>103</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A128" t="s">
-        <v>106</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="54" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="27" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
+        <v>174</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>107</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="27" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>108</v>
       </c>
-      <c r="E131" s="3" t="s">
+      <c r="E133" s="3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="108" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
+    <row r="134" spans="1:5" ht="108" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>115</v>
       </c>
-      <c r="E132" s="3" t="s">
+      <c r="E134" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="81" x14ac:dyDescent="0.35">
-      <c r="A133" t="s">
+    <row r="135" spans="1:5" ht="81" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>116</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C135" t="s">
         <v>191</v>
       </c>
-      <c r="E133" s="3" t="s">
+      <c r="E135" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="81" x14ac:dyDescent="0.35">
-      <c r="A134" t="s">
+    <row r="136" spans="1:5" ht="81" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>117</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C136" t="s">
         <v>191</v>
       </c>
-      <c r="E134" s="3" t="s">
+      <c r="E136" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="67.5" x14ac:dyDescent="0.35">
-      <c r="A135" t="s">
+    <row r="137" spans="1:5" ht="67.5" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>118</v>
       </c>
-      <c r="E135" s="3" t="s">
+      <c r="E137" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="A136" t="s">
+    <row r="138" spans="1:5" ht="13.9" x14ac:dyDescent="0.4">
+      <c r="A138" t="s">
         <v>119</v>
       </c>
-      <c r="C136" s="6" t="s">
+      <c r="C138" s="6" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A137" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>